<commit_message>
Solved most of 01
</commit_message>
<xml_diff>
--- a/01/hü_170315_moritz_goeckel.xlsx
+++ b/01/hü_170315_moritz_goeckel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="270" windowWidth="18540" windowHeight="8390"/>
+    <workbookView xWindow="480" yWindow="270" windowWidth="18540" windowHeight="8390" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Beispielprojekt_1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>Nr.</t>
   </si>
@@ -174,17 +174,24 @@
   </si>
   <si>
     <t>Uhrzeit</t>
+  </si>
+  <si>
+    <t>Quartal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;€&quot;\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="&quot;€&quot;\ #,##0.000"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$€]_-;\-* #,##0.00\ [$€]_-;_-* &quot;-&quot;??\ [$€]_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="h:mm;@"/>
+    <numFmt numFmtId="172" formatCode="#\ ???/???"/>
+    <numFmt numFmtId="174" formatCode="#,##0.000\ &quot;€&quot;"/>
+    <numFmt numFmtId="175" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -240,7 +247,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +263,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="52"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,7 +394,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -418,12 +431,6 @@
     </xf>
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
@@ -446,12 +453,32 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="4" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="174" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Euro" xfId="1"/>
@@ -460,57 +487,7 @@
     <cellStyle name="Standard 2" xfId="3"/>
     <cellStyle name="Standard_Tabelle2" xfId="4"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -533,41 +510,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -873,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -934,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="4">
-        <f>D5+E5</f>
+        <f>WORKDAY(D5,E5,Feiertage!$A$2:$A$6)</f>
         <v>42782</v>
       </c>
       <c r="G5" s="11">
@@ -959,8 +906,8 @@
         <v>10</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" ref="F6:F12" ca="1" si="0">D6+E6</f>
-        <v>42792</v>
+        <f ca="1">WORKDAY(D6,E6,Feiertage!$A$2:$A$6)</f>
+        <v>42796</v>
       </c>
       <c r="G6" s="11">
         <v>1</v>
@@ -977,15 +924,15 @@
         <v>7</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" ref="D7:D12" ca="1" si="1">INDIRECT("F"&amp;B7 + 4)</f>
+        <f t="shared" ref="D7:D11" ca="1" si="0">INDIRECT("F"&amp;B7 + 4)</f>
         <v>42782</v>
       </c>
       <c r="E7" s="3">
         <v>4</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>42786</v>
+        <f ca="1">WORKDAY(D7,E7,Feiertage!$A$2:$A$6)</f>
+        <v>42788</v>
       </c>
       <c r="G7" s="11">
         <v>1</v>
@@ -1002,15 +949,15 @@
         <v>8</v>
       </c>
       <c r="D8" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>42786</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>42788</v>
       </c>
       <c r="E8" s="3">
         <v>8</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>42794</v>
+        <f ca="1">WORKDAY(D8,E8,Feiertage!$A$2:$A$6)</f>
+        <v>42800</v>
       </c>
       <c r="G8" s="11">
         <v>1</v>
@@ -1027,15 +974,15 @@
         <v>9</v>
       </c>
       <c r="D9" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>42794</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>42800</v>
       </c>
       <c r="E9" s="3">
         <v>10</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>42804</v>
+        <f ca="1">WORKDAY(D9,E9,Feiertage!$A$2:$A$6)</f>
+        <v>42814</v>
       </c>
       <c r="G9" s="11">
         <v>0.8</v>
@@ -1052,20 +999,20 @@
         <v>10</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>42794</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>42800</v>
       </c>
       <c r="E10" s="3">
         <v>21</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>42815</v>
+        <f ca="1">WORKDAY(D10,E10,Feiertage!$A$2:$A$6)</f>
+        <v>42829</v>
       </c>
       <c r="G10" s="11">
         <v>0.5</v>
       </c>
-      <c r="L10" s="41"/>
+      <c r="L10" s="38"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -1078,15 +1025,15 @@
         <v>11</v>
       </c>
       <c r="D11" s="4">
-        <f t="shared" ca="1" si="1"/>
-        <v>42815</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>42829</v>
       </c>
       <c r="E11" s="3">
         <v>13</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>42828</v>
+        <f ca="1">WORKDAY(D11,E11,Feiertage!$A$2:$A$6)</f>
+        <v>42849</v>
       </c>
       <c r="G11" s="11">
         <v>0</v>
@@ -1104,14 +1051,14 @@
       </c>
       <c r="D12" s="4">
         <f ca="1">INDIRECT("F"&amp;B12 + 4)</f>
-        <v>42828</v>
+        <v>42849</v>
       </c>
       <c r="E12" s="3">
         <v>15</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>42843</v>
+        <f ca="1">WORKDAY(D12,E12,Feiertage!$A$2:$A$6)</f>
+        <v>42871</v>
       </c>
       <c r="G12" s="11">
         <v>0</v>
@@ -1173,15 +1120,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G5:G12">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThanOrEqual">
-      <formula>0.75</formula>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+      <formula>0.35</formula>
+      <formula>0.74</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0.35</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
-      <formula>0.35</formula>
-      <formula>0.74</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThanOrEqual">
+      <formula>0.75</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1263,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1313,9 +1260,23 @@
       <c r="D2" s="16">
         <v>0.65625</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="E2" s="40">
+        <f>D2-C2</f>
+        <v>0.28125</v>
+      </c>
+      <c r="F2" s="41">
+        <f>IF(E2&gt;10/24,E2 - 1 / 24, IF(E2 &gt; 8 / 24, E2 - 1 / 2 / 24, E2))</f>
+        <v>0.28125</v>
+      </c>
       <c r="G2" s="18"/>
+      <c r="H2" s="42">
+        <f>CEILING(MONTH(A2) / 12 * 4, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="45">
+        <f>IF(H2=$F$27, F2, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
@@ -1330,8 +1291,22 @@
       <c r="D3" s="16">
         <v>0.71875</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="E3" s="40">
+        <f>D3-C3</f>
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="F3" s="41">
+        <f>IF(E3&gt;10/24,E3 - 1 / 24, IF(E3 &gt; 8 / 24, E3 - 1 / 2 / 24, E3))</f>
+        <v>0.34375</v>
+      </c>
+      <c r="H3" s="42">
+        <f t="shared" ref="H3:H24" si="0">CEILING(MONTH(A3) / 12 * 4, 1)</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="45">
+        <f t="shared" ref="I3:I24" si="1">IF(H3=$F$27, F3, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
@@ -1346,8 +1321,22 @@
       <c r="D4" s="16">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
+      <c r="E4" s="40">
+        <f>D4-C4</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F4" s="41">
+        <f>IF(E4&gt;10/24,E4 - 1 / 24, IF(E4 &gt; 8 / 24, E4 - 1 / 2 / 24, E4))</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H4" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I4" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
@@ -1362,8 +1351,22 @@
       <c r="D5" s="16">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
+      <c r="E5" s="40">
+        <f>D5-C5</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F5" s="41">
+        <f>IF(E5&gt;10/24,E5 - 1 / 24, IF(E5 &gt; 8 / 24, E5 - 1 / 2 / 24, E5))</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H5" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I5" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
@@ -1378,8 +1381,22 @@
       <c r="D6" s="16">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+      <c r="E6" s="40">
+        <f>D6-C6</f>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="F6" s="41">
+        <f>IF(E6&gt;10/24,E6 - 1 / 24, IF(E6 &gt; 8 / 24, E6 - 1 / 2 / 24, E6))</f>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="H6" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
@@ -1394,8 +1411,22 @@
       <c r="D7" s="16">
         <v>0.625</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
+      <c r="E7" s="40">
+        <f>D7-C7</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F7" s="41">
+        <f>IF(E7&gt;10/24,E7 - 1 / 24, IF(E7 &gt; 8 / 24, E7 - 1 / 2 / 24, E7))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H7" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
@@ -1410,8 +1441,22 @@
       <c r="D8" s="16">
         <v>0.6875</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
+      <c r="E8" s="40">
+        <f>D8-C8</f>
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F8" s="41">
+        <f>IF(E8&gt;10/24,E8 - 1 / 24, IF(E8 &gt; 8 / 24, E8 - 1 / 2 / 24, E8))</f>
+        <v>0.375</v>
+      </c>
+      <c r="H8" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I8" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
@@ -1426,8 +1471,22 @@
       <c r="D9" s="16">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
+      <c r="E9" s="40">
+        <f>D9-C9</f>
+        <v>0.18749999999999994</v>
+      </c>
+      <c r="F9" s="41">
+        <f>IF(E9&gt;10/24,E9 - 1 / 24, IF(E9 &gt; 8 / 24, E9 - 1 / 2 / 24, E9))</f>
+        <v>0.18749999999999994</v>
+      </c>
+      <c r="H9" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
@@ -1442,8 +1501,22 @@
       <c r="D10" s="16">
         <v>0.69791666666666663</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
+      <c r="E10" s="40">
+        <f>D10-C10</f>
+        <v>0.31249999999999994</v>
+      </c>
+      <c r="F10" s="41">
+        <f>IF(E10&gt;10/24,E10 - 1 / 24, IF(E10 &gt; 8 / 24, E10 - 1 / 2 / 24, E10))</f>
+        <v>0.31249999999999994</v>
+      </c>
+      <c r="H10" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I10" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
@@ -1458,8 +1531,22 @@
       <c r="D11" s="16">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="E11" s="40">
+        <f>D11-C11</f>
+        <v>0.20833333333333326</v>
+      </c>
+      <c r="F11" s="41">
+        <f>IF(E11&gt;10/24,E11 - 1 / 24, IF(E11 &gt; 8 / 24, E11 - 1 / 2 / 24, E11))</f>
+        <v>0.20833333333333326</v>
+      </c>
+      <c r="H11" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I11" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
@@ -1474,8 +1561,22 @@
       <c r="D12" s="16">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
+      <c r="E12" s="40">
+        <f>D12-C12</f>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="F12" s="41">
+        <f>IF(E12&gt;10/24,E12 - 1 / 24, IF(E12 &gt; 8 / 24, E12 - 1 / 2 / 24, E12))</f>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="H12" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
@@ -1490,8 +1591,22 @@
       <c r="D13" s="16">
         <v>0.5</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
+      <c r="E13" s="40">
+        <f>D13-C13</f>
+        <v>0.125</v>
+      </c>
+      <c r="F13" s="41">
+        <f>IF(E13&gt;10/24,E13 - 1 / 24, IF(E13 &gt; 8 / 24, E13 - 1 / 2 / 24, E13))</f>
+        <v>0.125</v>
+      </c>
+      <c r="H13" s="42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I13" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
@@ -1506,8 +1621,22 @@
       <c r="D14" s="16">
         <v>0.625</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
+      <c r="E14" s="40">
+        <f>D14-C14</f>
+        <v>0.25</v>
+      </c>
+      <c r="F14" s="41">
+        <f>IF(E14&gt;10/24,E14 - 1 / 24, IF(E14 &gt; 8 / 24, E14 - 1 / 2 / 24, E14))</f>
+        <v>0.25</v>
+      </c>
+      <c r="H14" s="42">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I14" s="45">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
@@ -1522,8 +1651,22 @@
       <c r="D15" s="16">
         <v>0.64583333333333337</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
+      <c r="E15" s="40">
+        <f>D15-C15</f>
+        <v>0.31250000000000006</v>
+      </c>
+      <c r="F15" s="41">
+        <f>IF(E15&gt;10/24,E15 - 1 / 24, IF(E15 &gt; 8 / 24, E15 - 1 / 2 / 24, E15))</f>
+        <v>0.31250000000000006</v>
+      </c>
+      <c r="H15" s="42">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I15" s="45">
+        <f t="shared" si="1"/>
+        <v>0.31250000000000006</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
@@ -1538,10 +1681,24 @@
       <c r="D16" s="16">
         <v>0.75</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-    </row>
-    <row r="17" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="40">
+        <f>D16-C16</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F16" s="41">
+        <f>IF(E16&gt;10/24,E16 - 1 / 24, IF(E16 &gt; 8 / 24, E16 - 1 / 2 / 24, E16))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H16" s="42">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I16" s="45">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
         <v>41396</v>
       </c>
@@ -1554,11 +1711,25 @@
       <c r="D17" s="16">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
+      <c r="E17" s="40">
+        <f>D17-C17</f>
+        <v>0.22916666666666669</v>
+      </c>
+      <c r="F17" s="41">
+        <f>IF(E17&gt;10/24,E17 - 1 / 24, IF(E17 &gt; 8 / 24, E17 - 1 / 2 / 24, E17))</f>
+        <v>0.22916666666666669</v>
+      </c>
       <c r="G17" s="19"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="42">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I17" s="45">
+        <f t="shared" si="1"/>
+        <v>0.22916666666666669</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>41428</v>
       </c>
@@ -1571,10 +1742,24 @@
       <c r="D18" s="16">
         <v>0.55208333333333337</v>
       </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="40">
+        <f>D18-C18</f>
+        <v>0.26041666666666669</v>
+      </c>
+      <c r="F18" s="41">
+        <f>IF(E18&gt;10/24,E18 - 1 / 24, IF(E18 &gt; 8 / 24, E18 - 1 / 2 / 24, E18))</f>
+        <v>0.26041666666666669</v>
+      </c>
+      <c r="H18" s="42">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I18" s="45">
+        <f t="shared" si="1"/>
+        <v>0.26041666666666669</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>41466</v>
       </c>
@@ -1587,10 +1772,24 @@
       <c r="D19" s="16">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="40">
+        <f>D19-C19</f>
+        <v>0.29166666666666663</v>
+      </c>
+      <c r="F19" s="41">
+        <f>IF(E19&gt;10/24,E19 - 1 / 24, IF(E19 &gt; 8 / 24, E19 - 1 / 2 / 24, E19))</f>
+        <v>0.29166666666666663</v>
+      </c>
+      <c r="H19" s="42">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I19" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>41475</v>
       </c>
@@ -1603,10 +1802,24 @@
       <c r="D20" s="16">
         <v>0.70833333333333337</v>
       </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="40">
+        <f>D20-C20</f>
+        <v>0.37500000000000006</v>
+      </c>
+      <c r="F20" s="41">
+        <f>IF(E20&gt;10/24,E20 - 1 / 24, IF(E20 &gt; 8 / 24, E20 - 1 / 2 / 24, E20))</f>
+        <v>0.35416666666666674</v>
+      </c>
+      <c r="H20" s="42">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I20" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>41551</v>
       </c>
@@ -1619,10 +1832,24 @@
       <c r="D21" s="16">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="40">
+        <f>D21-C21</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="F21" s="41">
+        <f>IF(E21&gt;10/24,E21 - 1 / 24, IF(E21 &gt; 8 / 24, E21 - 1 / 2 / 24, E21))</f>
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="H21" s="42">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I21" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>41552</v>
       </c>
@@ -1635,10 +1862,24 @@
       <c r="D22" s="16">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="40">
+        <f>D22-C22</f>
+        <v>0.24999999999999994</v>
+      </c>
+      <c r="F22" s="41">
+        <f>IF(E22&gt;10/24,E22 - 1 / 24, IF(E22 &gt; 8 / 24, E22 - 1 / 2 / 24, E22))</f>
+        <v>0.24999999999999994</v>
+      </c>
+      <c r="H22" s="42">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I22" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>41583</v>
       </c>
@@ -1651,10 +1892,24 @@
       <c r="D23" s="16">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="40">
+        <f>D23-C23</f>
+        <v>0.24999999999999994</v>
+      </c>
+      <c r="F23" s="41">
+        <f>IF(E23&gt;10/24,E23 - 1 / 24, IF(E23 &gt; 8 / 24, E23 - 1 / 2 / 24, E23))</f>
+        <v>0.24999999999999994</v>
+      </c>
+      <c r="H23" s="42">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I23" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>41588</v>
       </c>
@@ -1667,26 +1922,48 @@
       <c r="D24" s="16">
         <v>0.875</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="40">
+        <f>D24-C24</f>
+        <v>0.5</v>
+      </c>
+      <c r="F24" s="41">
+        <f>IF(E24&gt;10/24,E24 - 1 / 24, IF(E24 &gt; 8 / 24, E24 - 1 / 2 / 24, E24))</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H24" s="42">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I24" s="45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="C27" s="13"/>
-      <c r="F27" s="20"/>
-    </row>
-    <row r="28" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+      <c r="D27" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="C28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="21"/>
+      <c r="F28" s="46">
+        <f>SUM(I2:I24)*24</f>
+        <v>33.25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -1695,8 +1972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1712,256 +1989,340 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24">
+      <c r="B1" s="21"/>
+      <c r="C1" s="22">
         <v>26.4</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="13" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24">
+      <c r="B2" s="21"/>
+      <c r="C2" s="22">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="25">
+      <c r="B3" s="21"/>
+      <c r="C3" s="23">
         <v>0.35599999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40" t="s">
+      <c r="B9" s="39"/>
+      <c r="C9" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="26" t="s">
+      <c r="D9" s="39"/>
+      <c r="E9" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="J9" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="K9" s="22" t="s">
+      <c r="K9" s="20" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="31"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E11" s="32"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="34"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="32"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="35">
+      <c r="A12" s="33">
         <v>41699</v>
       </c>
-      <c r="B12" s="36">
+      <c r="B12" s="34">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="33">
         <v>41699</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="34">
         <v>0.70833333333333304</v>
       </c>
-      <c r="E12" s="37">
+      <c r="E12" s="35">
         <v>745</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
+      <c r="F12" s="47">
+        <f xml:space="preserve"> (C12 + D12) - (A12+B12)</f>
+        <v>0.375</v>
+      </c>
+      <c r="G12" s="36">
+        <f>F12 * 24</f>
+        <v>9</v>
+      </c>
+      <c r="H12" s="36"/>
+      <c r="I12" s="48">
+        <f>$C$3*E12</f>
+        <v>265.21999999999997</v>
+      </c>
+      <c r="J12" s="36"/>
+      <c r="K12" s="49">
+        <f>IF(F12&gt;=1,$C$2,0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="35">
+      <c r="A13" s="33">
         <v>41700</v>
       </c>
-      <c r="B13" s="36">
+      <c r="B13" s="34">
         <v>0.25</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="33">
         <v>41701</v>
       </c>
-      <c r="D13" s="36">
+      <c r="D13" s="34">
         <v>0.625</v>
       </c>
-      <c r="E13" s="37">
+      <c r="E13" s="35">
         <v>1623</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
+      <c r="F13" s="47">
+        <f xml:space="preserve"> (C13 + D13) - (A13+B13)</f>
+        <v>1.375</v>
+      </c>
+      <c r="G13" s="36">
+        <f>F13 * 24</f>
+        <v>33</v>
+      </c>
+      <c r="H13" s="36"/>
+      <c r="I13" s="48">
+        <f>$C$3*E13</f>
+        <v>577.78800000000001</v>
+      </c>
+      <c r="J13" s="36"/>
+      <c r="K13" s="49">
+        <f t="shared" ref="K13:K18" si="0">IF(F13&gt;=1,$C$2,0)</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="35">
+      <c r="A14" s="33">
         <v>41703</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="34">
         <v>0.375</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="33">
         <v>41703</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="34">
         <v>0.54166666666666696</v>
       </c>
-      <c r="E14" s="37">
+      <c r="E14" s="35">
         <v>67</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
+      <c r="F14" s="47">
+        <f xml:space="preserve"> (C14 + D14) - (A14+B14)</f>
+        <v>0.16666666666424135</v>
+      </c>
+      <c r="G14" s="36">
+        <f>F14 * 24</f>
+        <v>3.9999999999417923</v>
+      </c>
+      <c r="H14" s="36"/>
+      <c r="I14" s="48">
+        <f>$C$3*E14</f>
+        <v>23.852</v>
+      </c>
+      <c r="J14" s="36"/>
+      <c r="K14" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="35">
+      <c r="A15" s="33">
         <v>41706</v>
       </c>
-      <c r="B15" s="36">
+      <c r="B15" s="34">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="33">
         <v>41707</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D15" s="34">
         <v>0.70833333333333304</v>
       </c>
-      <c r="E15" s="37">
+      <c r="E15" s="35">
         <v>2012</v>
       </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
+      <c r="F15" s="47">
+        <f xml:space="preserve"> (C15 + D15) - (A15+B15)</f>
+        <v>1.375</v>
+      </c>
+      <c r="G15" s="36">
+        <f>F15 * 24</f>
+        <v>33</v>
+      </c>
+      <c r="H15" s="36"/>
+      <c r="I15" s="48">
+        <f>$C$3*E15</f>
+        <v>716.27199999999993</v>
+      </c>
+      <c r="J15" s="36"/>
+      <c r="K15" s="49">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="35">
+      <c r="A16" s="33">
         <v>41710</v>
       </c>
-      <c r="B16" s="36">
+      <c r="B16" s="34">
         <v>0.41666666666666702</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="33">
         <v>41710</v>
       </c>
-      <c r="D16" s="36">
+      <c r="D16" s="34">
         <v>0.95833333333333304</v>
       </c>
-      <c r="E16" s="37">
+      <c r="E16" s="35">
         <v>134</v>
       </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="38"/>
+      <c r="F16" s="47">
+        <f xml:space="preserve"> (C16 + D16) - (A16+B16)</f>
+        <v>0.54166666667151731</v>
+      </c>
+      <c r="G16" s="36">
+        <f>F16 * 24</f>
+        <v>13.000000000116415</v>
+      </c>
+      <c r="H16" s="36"/>
+      <c r="I16" s="48">
+        <f>$C$3*E16</f>
+        <v>47.704000000000001</v>
+      </c>
+      <c r="J16" s="36"/>
+      <c r="K16" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="35">
+      <c r="A17" s="33">
         <v>41713</v>
       </c>
-      <c r="B17" s="36">
+      <c r="B17" s="34">
         <v>0.375</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="33">
         <v>41713</v>
       </c>
-      <c r="D17" s="36">
+      <c r="D17" s="34">
         <v>0.45833333333333298</v>
       </c>
-      <c r="E17" s="37">
+      <c r="E17" s="35">
         <v>13</v>
       </c>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="F17" s="47">
+        <f xml:space="preserve"> (C17 + D17) - (A17+B17)</f>
+        <v>8.3333333335758653E-2</v>
+      </c>
+      <c r="G17" s="36">
+        <f>F17 * 24</f>
+        <v>2.0000000000582077</v>
+      </c>
+      <c r="H17" s="36"/>
+      <c r="I17" s="48">
+        <f>$C$3*E17</f>
+        <v>4.6280000000000001</v>
+      </c>
+      <c r="J17" s="36"/>
+      <c r="K17" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="35">
+      <c r="A18" s="33">
         <v>41717</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="34">
         <v>0.20833333333333301</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C18" s="33">
         <v>41717</v>
       </c>
-      <c r="D18" s="36">
+      <c r="D18" s="34">
         <v>0.54166666666666696</v>
       </c>
-      <c r="E18" s="37">
+      <c r="E18" s="35">
         <v>462</v>
       </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="F18" s="47">
+        <f xml:space="preserve"> (C18 + D18) - (A18+B18)</f>
+        <v>0.33333333332848269</v>
+      </c>
+      <c r="G18" s="36">
+        <f>F18 * 24</f>
+        <v>7.9999999998835847</v>
+      </c>
+      <c r="H18" s="36"/>
+      <c r="I18" s="48">
+        <f>$C$3*E18</f>
+        <v>164.47199999999998</v>
+      </c>
+      <c r="J18" s="36"/>
+      <c r="K18" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H20" s="39"/>
+      <c r="H20" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>